<commit_message>
functional GUI with dummy data
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ASUS\python\hexachase\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C14C83C4-E3B0-4827-9923-1C5259EA5BB7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1C8EE52C-29CA-47FB-9561-CCC4B6AAB457}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{2E6563A6-70CC-4FF3-A143-89544E765E66}"/>
   </bookViews>
@@ -430,7 +430,7 @@
   <dimension ref="A1:D11"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G6" sqref="G6"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>